<commit_message>
Fixed formula9 in benchmark
</commit_message>
<xml_diff>
--- a/BenchResults/Benchmark.xlsx
+++ b/BenchResults/Benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkovtun\source\repos\NoStringEvaluating\BenchResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5464166-D20D-4179-AD1A-6713D57A972B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A7A518-7B68-44B4-BE49-63E1D2BE80A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,10 +87,10 @@
     <t>Arg1 * (Arg2 + Arg3) - Arg4 / (Arg5 - Arg6) + 45 * Arg7 + ((Arg8 * 56 + (12 + Arg9))) - Arg10</t>
   </si>
   <si>
-    <t>if(Arg1; add(56 + 9 / 12 * 123.596; or(78; 9; 5; 2; 4; 5; 8; 7); 45;5); 9) *     24 + 52 -33</t>
+    <t>Allocated, KB</t>
   </si>
   <si>
-    <t>Allocated, KB</t>
+    <t>if(Arg1 &gt; 0; add(56 + 9 / 12 * 123.596; or(78; 9; 5; 2; 4; 5; 8; 7); 45;5); 9) *     24 + 52 -33</t>
   </si>
 </sst>
 </file>
@@ -227,6 +227,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -235,15 +244,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1727,7 +1727,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B5:U75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:U13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1748,370 +1750,370 @@
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
     </row>
     <row r="6" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
     </row>
     <row r="7" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="14">
         <v>3</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="12"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
     </row>
     <row r="8" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C8" s="3">
         <v>1</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="12"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
     </row>
     <row r="9" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C9" s="3">
         <v>2</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="12"/>
-      <c r="U9" s="12"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
     </row>
     <row r="10" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>3</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
     </row>
     <row r="11" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>4</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
     </row>
     <row r="12" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>5</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="12"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
     </row>
     <row r="13" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C13" s="3">
         <v>6</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
     </row>
     <row r="14" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C14" s="3">
         <v>7</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="12"/>
-      <c r="U14" s="12"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
     </row>
     <row r="15" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <v>8</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="12"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
-      <c r="U15" s="12"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15"/>
     </row>
     <row r="16" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C16" s="3">
         <v>9</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
-      <c r="U16" s="12"/>
+      <c r="D16" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C17" s="3">
         <v>10</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="12"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="16"/>
-      <c r="S19" s="16"/>
-      <c r="T19" s="16"/>
-      <c r="U19" s="16"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="15"/>
+      <c r="E20" s="11"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
-      <c r="I20" s="15" t="s">
+      <c r="I20" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="J20" s="15"/>
+      <c r="J20" s="11"/>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="C21" s="14"/>
+      <c r="C21" s="13"/>
       <c r="D21" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
@@ -2119,7 +2121,7 @@
         <v>13</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.3">
@@ -2440,11 +2442,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="C19:U19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D17:U17"/>
     <mergeCell ref="D16:U16"/>
     <mergeCell ref="D5:U5"/>
     <mergeCell ref="D6:U6"/>
@@ -2457,6 +2454,11 @@
     <mergeCell ref="D13:U13"/>
     <mergeCell ref="D14:U14"/>
     <mergeCell ref="D15:U15"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="C19:U19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D17:U17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated to improved mXparser version
</commit_message>
<xml_diff>
--- a/BenchResults/Benchmark.xlsx
+++ b/BenchResults/Benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkovtun\source\repos\NoStringEvaluating\BenchResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A7A518-7B68-44B4-BE49-63E1D2BE80A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA451DC2-BBC2-4CA4-8786-37C641F04EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -409,40 +409,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>105</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>106</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>181</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1064</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1324</c:v>
+                  <c:v>597</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9849</c:v>
+                  <c:v>2552</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>512</c:v>
+                  <c:v>352</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3402</c:v>
+                  <c:v>1342</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>521</c:v>
+                  <c:v>323</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1487</c:v>
+                  <c:v>695</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4512</c:v>
+                  <c:v>8567</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1270</c:v>
+                  <c:v>717</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -520,40 +520,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>44</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>113</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>112</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>343</c:v>
+                  <c:v>351</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>161</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>359</c:v>
+                  <c:v>370</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>279</c:v>
+                  <c:v>284</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>600</c:v>
+                  <c:v>622</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>251</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1727,9 +1727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B5:U75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:U13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2129,7 +2127,7 @@
         <v>7</v>
       </c>
       <c r="D22" s="2">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E22" s="2">
         <v>406250</v>
@@ -2137,10 +2135,10 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2">
         <f>ROUND(D22/I22, 0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I22" s="10">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="J22" s="2">
         <v>3</v>
@@ -2151,7 +2149,7 @@
         <v>8</v>
       </c>
       <c r="D23" s="2">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E23" s="2">
         <v>148515</v>
@@ -2162,7 +2160,7 @@
         <v>2</v>
       </c>
       <c r="I23" s="2">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J23" s="2">
         <v>4</v>
@@ -2174,7 +2172,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="2">
-        <v>181</v>
+        <v>143</v>
       </c>
       <c r="E24" s="2">
         <v>273523</v>
@@ -2182,10 +2180,10 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I24" s="2">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J24" s="2">
         <v>4</v>
@@ -2197,18 +2195,18 @@
         <v>2</v>
       </c>
       <c r="D25" s="2">
-        <v>1064</v>
+        <v>480</v>
       </c>
       <c r="E25" s="2">
-        <v>1133047</v>
+        <v>1133048</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I25" s="2">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="J25" s="2">
         <v>4</v>
@@ -2220,7 +2218,7 @@
         <v>3</v>
       </c>
       <c r="D26" s="2">
-        <v>1324</v>
+        <v>597</v>
       </c>
       <c r="E26" s="2">
         <v>1656536</v>
@@ -2228,10 +2226,10 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I26" s="2">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="J26" s="2">
         <v>5</v>
@@ -2243,18 +2241,18 @@
         <v>4</v>
       </c>
       <c r="D27" s="2">
-        <v>9849</v>
+        <v>2552</v>
       </c>
       <c r="E27" s="2">
-        <v>6954197</v>
+        <v>6954199</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="I27" s="2">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="J27" s="2">
         <v>10</v>
@@ -2266,18 +2264,18 @@
         <v>5</v>
       </c>
       <c r="D28" s="2">
-        <v>512</v>
+        <v>352</v>
       </c>
       <c r="E28" s="2">
-        <v>609593</v>
+        <v>609594</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I28" s="2">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J28" s="2">
         <v>5</v>
@@ -2290,18 +2288,18 @@
         <v>6</v>
       </c>
       <c r="D29" s="2">
-        <v>3402</v>
+        <v>1342</v>
       </c>
       <c r="E29" s="2">
-        <v>3305393</v>
+        <v>3305395</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I29" s="2">
-        <v>359</v>
+        <v>370</v>
       </c>
       <c r="J29" s="2">
         <v>8</v>
@@ -2314,15 +2312,15 @@
         <v>7</v>
       </c>
       <c r="D30" s="2">
-        <v>521</v>
+        <v>323</v>
       </c>
       <c r="E30" s="2">
-        <v>875129</v>
+        <v>804816</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I30" s="2">
         <v>149</v>
@@ -2338,18 +2336,18 @@
         <v>8</v>
       </c>
       <c r="D31" s="2">
-        <v>1487</v>
+        <v>695</v>
       </c>
       <c r="E31" s="2">
-        <v>2234638</v>
+        <v>2094014</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I31" s="2">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="J31" s="2">
         <v>7</v>
@@ -2362,18 +2360,18 @@
         <v>9</v>
       </c>
       <c r="D32" s="5">
-        <v>4512</v>
+        <v>8567</v>
       </c>
       <c r="E32" s="2">
-        <v>7570919</v>
+        <v>9360871</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="I32" s="2">
-        <v>600</v>
+        <v>622</v>
       </c>
       <c r="J32" s="2">
         <v>11</v>
@@ -2386,18 +2384,18 @@
         <v>10</v>
       </c>
       <c r="D33" s="5">
-        <v>1270</v>
+        <v>717</v>
       </c>
       <c r="E33" s="5">
-        <v>1656470</v>
+        <v>1515846</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I33" s="2">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J33" s="2">
         <v>6</v>
@@ -2408,7 +2406,7 @@
       <c r="B34" s="6"/>
       <c r="G34" s="2" t="str">
         <f>_xlfn.CONCAT("x", ROUND(AVERAGE(G22:G33), 0))</f>
-        <v>x8</v>
+        <v>x4</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.3">

</xml_diff>